<commit_message>
Fixed Matlab memory leak, finished 10 tests
</commit_message>
<xml_diff>
--- a/results/Zeszyt1.xlsx
+++ b/results/Zeszyt1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakub Burczyk\Documents\PycharmProjects\guiio_pid_tuner\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E84994-4096-48F2-8A09-64832C81FFD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98727561-7A08-4237-90FB-BDD2A1BBF8D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FB000F19-9E91-4619-9DA7-216F5506CF56}"/>
   </bookViews>
@@ -411,7 +411,7 @@
   <dimension ref="B2:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,15 +674,51 @@
       <c r="I12">
         <v>8</v>
       </c>
+      <c r="J12">
+        <v>1.2E-2</v>
+      </c>
+      <c r="K12">
+        <v>0.109</v>
+      </c>
+      <c r="L12">
+        <v>11.96</v>
+      </c>
+      <c r="M12">
+        <v>6.7880000000000003</v>
+      </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I13">
         <v>9</v>
       </c>
+      <c r="J13">
+        <v>2E-3</v>
+      </c>
+      <c r="K13">
+        <v>0.185</v>
+      </c>
+      <c r="L13">
+        <v>12</v>
+      </c>
+      <c r="M13">
+        <v>6.8609999999999998</v>
+      </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I14">
         <v>10</v>
+      </c>
+      <c r="J14">
+        <v>54.73</v>
+      </c>
+      <c r="K14">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="L14">
+        <v>12.06</v>
+      </c>
+      <c r="M14">
+        <v>8.3800000000000008</v>
       </c>
     </row>
   </sheetData>

</xml_diff>